<commit_message>
Fix some failing tests.
</commit_message>
<xml_diff>
--- a/src/Tests/RegressionTests/Expected/RecordInstanceHorizontal.xlsx
+++ b/src/Tests/RegressionTests/Expected/RecordInstanceHorizontal.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:si>
     <x:t>Name</x:t>
   </x:si>
@@ -29,6 +29,9 @@
   </x:si>
   <x:si>
     <x:t>Jane Smith</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2022-03-12</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -37,7 +40,7 @@
 <x:styleSheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:numFmts count="2">
     <x:numFmt numFmtId="0" formatCode=""/>
-    <x:numFmt numFmtId="165" formatCode="$0.00"/>
+    <x:numFmt numFmtId="164" formatCode="$0.00"/>
   </x:numFmts>
   <x:fonts count="2">
     <x:font>
@@ -100,21 +103,18 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="4">
+  <x:cellStyleXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="4">
+  <x:cellXfs count="3">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -123,11 +123,7 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -432,13 +428,13 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="11.050625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="5.160625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="7.680625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="11.610625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="11.140625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="5.110625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="7.730625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="11.400625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" customFormat="1" ht="15.218096" customHeight="1">
+    <x:row r="1" spans="1:4" ht="13.75" customHeight="1">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -452,18 +448,18 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" customFormat="1" ht="15.218096" customHeight="1">
+    <x:row r="2" spans="1:4" ht="13.75" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="n">
+      <x:c r="B2" s="0">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="C2" s="2" t="n">
+      <x:c r="C2" s="2">
         <x:v>59.25</x:v>
       </x:c>
-      <x:c r="D2" s="3">
-        <x:v>44632</x:v>
+      <x:c r="D2" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>